<commit_message>
added clearer char1,png and HED.png and link to proper css in hed\addenda\index.htm
</commit_message>
<xml_diff>
--- a/hed/addenda/addendum.xlsx
+++ b/hed/addenda/addendum.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="121">
   <si>
     <t>ōt</t>
   </si>
@@ -508,6 +508,202 @@
       </rPr>
       <t>{Remove link in column D 繁}
 {Note: all bad links were corrected in in master 20230113}</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">𦉗 </t>
+  </si>
+  <si>
+    <t>hel5</t>
+  </si>
+  <si>
+    <t>hêl</t>
+  </si>
+  <si>
+    <t>pït</t>
+  </si>
+  <si>
+    <t>säk</t>
+  </si>
+  <si>
+    <t>缶</t>
+  </si>
+  <si>
+    <t>náo</t>
+  </si>
+  <si>
+    <t>yáo</t>
+  </si>
+  <si>
+    <t>𡒭</t>
+  </si>
+  <si>
+    <t>土</t>
+  </si>
+  <si>
+    <t>não</t>
+  </si>
+  <si>
+    <t>nao3</t>
+  </si>
+  <si>
+    <t>yẽl</t>
+  </si>
+  <si>
+    <t>yel3</t>
+  </si>
+  <si>
+    <t>lẽl</t>
+  </si>
+  <si>
+    <t>liáo</t>
+  </si>
+  <si>
+    <t>lel3</t>
+  </si>
+  <si>
+    <t>tiào</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Vietnamese pronunciation </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t>niêu</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">: a small casserole.¹¹³
+(composition: ⿰土僚; U+214AD).
+&lt;又&gt; hêl, não, yẽl. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t>(See 𦉗 hêl, 𦉗 não, 𦉗 yẽl.)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">found in Taiwanese names. Same as Vietnamese 𡒭 </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t>niêu</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">: a small casserole.¹¹³
+(composition: ⿰缶堯; U+26257).
+&lt;又&gt; hêl, lẽl, yẽl. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t>(See 𦉗 hêl, 𡒭 lẽl, 𦉗 yẽl.)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">found in Taiwanese names. Same as Vietnamese 𡒭 niêu: a small casserole.¹¹³
+(composition: ⿰缶堯; U+26257).
+&lt;又&gt; hêl, lẽl, não. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t>(See 𦉗 hêl, 𡒭 lẽl, 𦉗 não.)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">&lt;台&gt; 𦉗 hêl a large clay cooking pot.¹²¹ʼ⁰
+(composition: ⿰缶堯; U+26257).
+&lt;又&gt; lẽl, não, yẽl. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t>(See 𡒭 lẽl, 𦉗 não, 𦉗 yẽl.)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
     </r>
   </si>
 </sst>
@@ -515,7 +711,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="26">
+  <fonts count="27">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -670,6 +866,12 @@
       <color rgb="FFA5A5A5"/>
       <name val="Segoe UI"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color rgb="FF4D4E51"/>
+      <name val="SimSun"/>
     </font>
   </fonts>
   <fills count="2">
@@ -696,7 +898,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -813,6 +1015,9 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -830,14 +1035,14 @@
     <xdr:from>
       <xdr:col>10</xdr:col>
       <xdr:colOff>43962</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>234462</xdr:rowOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>234461</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
       <xdr:colOff>625068</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>825094</xdr:rowOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>740018</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -854,8 +1059,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7627327" y="1545981"/>
-          <a:ext cx="581106" cy="590632"/>
+          <a:off x="7649308" y="6931269"/>
+          <a:ext cx="581106" cy="505557"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1152,10 +1357,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N19"/>
+  <dimension ref="A1:N23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30.75"/>
@@ -1215,529 +1420,651 @@
       <c r="M1"/>
       <c r="N1"/>
     </row>
-    <row r="2" spans="1:14" ht="86.25">
+    <row r="2" spans="1:14" ht="51.75">
       <c r="A2" s="11">
-        <v>196</v>
-      </c>
-      <c r="B2" s="24" t="s">
-        <v>18</v>
+        <v>50</v>
+      </c>
+      <c r="B2" s="32" t="s">
+        <v>30</v>
       </c>
       <c r="C2" s="11">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="D2" s="25" t="s">
-        <v>19</v>
-      </c>
-      <c r="E2" s="26" t="s">
-        <v>20</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="E2" s="26"/>
       <c r="F2" s="27" t="s">
-        <v>21</v>
+        <v>32</v>
       </c>
       <c r="G2" s="28" t="s">
-        <v>22</v>
-      </c>
-      <c r="H2" s="30" t="s">
-        <v>40</v>
-      </c>
-      <c r="I2" s="31" t="s">
-        <v>23</v>
-      </c>
-      <c r="J2" s="23">
-        <v>4962</v>
-      </c>
-      <c r="K2" s="11"/>
+        <v>33</v>
+      </c>
+      <c r="H2" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="I2" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="J2" s="22">
+        <v>1515</v>
+      </c>
       <c r="L2"/>
       <c r="M2"/>
       <c r="N2"/>
     </row>
     <row r="3" spans="1:14" ht="110.25" customHeight="1">
       <c r="A3" s="11">
-        <v>85</v>
-      </c>
-      <c r="B3" s="24" t="s">
-        <v>24</v>
+        <v>6</v>
+      </c>
+      <c r="B3" s="32" t="s">
+        <v>35</v>
       </c>
       <c r="C3" s="11">
-        <v>15</v>
-      </c>
-      <c r="D3" s="25" t="s">
-        <v>25</v>
-      </c>
-      <c r="E3" s="26" t="s">
-        <v>25</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="D3" s="33" t="s">
+        <v>39</v>
+      </c>
+      <c r="E3" s="34"/>
       <c r="F3" s="27" t="s">
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="G3" s="28" t="s">
-        <v>27</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>41</v>
+        <v>37</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>43</v>
       </c>
       <c r="I3" s="29" t="s">
+        <v>38</v>
+      </c>
+      <c r="J3" s="11">
+        <v>1854</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" ht="61.5">
+      <c r="A4" s="11">
+        <v>66</v>
+      </c>
+      <c r="B4" s="32" t="s">
+        <v>35</v>
+      </c>
+      <c r="C4" s="11">
+        <v>13</v>
+      </c>
+      <c r="D4" s="33" t="s">
+        <v>44</v>
+      </c>
+      <c r="E4" s="34"/>
+      <c r="F4" s="27" t="s">
+        <v>36</v>
+      </c>
+      <c r="G4" s="28" t="s">
+        <v>37</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="I4" s="29" t="s">
+        <v>38</v>
+      </c>
+      <c r="J4" s="11">
+        <v>1855</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" ht="34.5">
+      <c r="A5" s="11">
+        <v>174</v>
+      </c>
+      <c r="B5" s="24" t="s">
+        <v>46</v>
+      </c>
+      <c r="C5" s="11">
+        <v>14</v>
+      </c>
+      <c r="D5" s="25" t="s">
+        <v>47</v>
+      </c>
+      <c r="E5" s="26"/>
+      <c r="F5" s="27" t="s">
+        <v>48</v>
+      </c>
+      <c r="G5" s="35" t="s">
+        <v>49</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="I5" s="29" t="s">
+        <v>50</v>
+      </c>
+      <c r="J5" s="11">
+        <v>2183</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" ht="86.25">
+      <c r="A6" s="11">
+        <v>196</v>
+      </c>
+      <c r="B6" s="24" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="11">
         <v>28</v>
       </c>
-      <c r="J3" s="11">
-        <v>15129</v>
-      </c>
-      <c r="K3" s="11" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14">
-      <c r="F4" s="14" t="s">
-        <v>0</v>
-      </c>
-      <c r="H4" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="I4" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="J4" s="5">
-        <v>90001</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" ht="34.5">
-      <c r="C5" s="23"/>
-      <c r="F5" s="15" t="s">
-        <v>3</v>
-      </c>
-      <c r="H5" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="I5" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="J5" s="5">
-        <v>90002</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14">
-      <c r="C6" s="23"/>
-      <c r="E6" s="20"/>
-      <c r="F6" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="H6" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="I6" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="J6" s="5">
-        <v>90003</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" ht="51.75">
+      <c r="D6" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="F6" s="27" t="s">
+        <v>21</v>
+      </c>
+      <c r="G6" s="28" t="s">
+        <v>22</v>
+      </c>
+      <c r="H6" s="30" t="s">
+        <v>40</v>
+      </c>
+      <c r="I6" s="31" t="s">
+        <v>23</v>
+      </c>
+      <c r="J6" s="23">
+        <v>4962</v>
+      </c>
+      <c r="K6" s="11"/>
+    </row>
+    <row r="7" spans="1:14" ht="34.5">
       <c r="A7" s="11">
-        <v>50</v>
+        <v>120</v>
       </c>
       <c r="B7" s="32" t="s">
-        <v>30</v>
+        <v>52</v>
       </c>
       <c r="C7" s="11">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="D7" s="25" t="s">
-        <v>31</v>
+        <v>53</v>
       </c>
       <c r="E7" s="26"/>
       <c r="F7" s="27" t="s">
-        <v>32</v>
+        <v>54</v>
       </c>
       <c r="G7" s="28" t="s">
-        <v>33</v>
-      </c>
-      <c r="H7" s="17" t="s">
-        <v>42</v>
-      </c>
-      <c r="I7" s="13" t="s">
-        <v>34</v>
+        <v>55</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="I7" s="31" t="s">
+        <v>56</v>
       </c>
       <c r="J7" s="22">
-        <v>1515</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" ht="69">
+        <v>5246</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" ht="34.5">
       <c r="A8" s="11">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="B8" s="32" t="s">
-        <v>35</v>
+        <v>57</v>
       </c>
       <c r="C8" s="11">
-        <v>13</v>
-      </c>
-      <c r="D8" s="33" t="s">
-        <v>39</v>
-      </c>
-      <c r="E8" s="34"/>
+        <v>4</v>
+      </c>
+      <c r="D8" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="E8" s="26"/>
       <c r="F8" s="27" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="G8" s="28" t="s">
-        <v>37</v>
+        <v>60</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="I8" s="29" t="s">
-        <v>38</v>
-      </c>
-      <c r="J8" s="11">
-        <v>1854</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" ht="61.5">
+        <v>45</v>
+      </c>
+      <c r="I8" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="J8" s="22">
+        <v>6498</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" ht="34.5">
       <c r="A9" s="11">
+        <v>26</v>
+      </c>
+      <c r="B9" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="C9" s="11">
+        <v>9</v>
+      </c>
+      <c r="D9" s="25" t="s">
+        <v>63</v>
+      </c>
+      <c r="E9" s="26"/>
+      <c r="F9" s="36" t="s">
+        <v>64</v>
+      </c>
+      <c r="G9" s="35" t="s">
+        <v>65</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="I9" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="B9" s="32" t="s">
-        <v>35</v>
-      </c>
-      <c r="C9" s="11">
-        <v>13</v>
-      </c>
-      <c r="D9" s="33" t="s">
-        <v>44</v>
-      </c>
-      <c r="E9" s="34"/>
-      <c r="F9" s="27" t="s">
-        <v>36</v>
-      </c>
-      <c r="G9" s="28" t="s">
-        <v>37</v>
-      </c>
-      <c r="H9" s="2" t="s">
+      <c r="J9" s="22">
+        <v>12089</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" ht="61.5">
+      <c r="A10" s="11">
+        <v>78</v>
+      </c>
+      <c r="B10" s="32" t="s">
+        <v>67</v>
+      </c>
+      <c r="C10" s="11">
+        <v>16</v>
+      </c>
+      <c r="D10" s="33" t="s">
+        <v>70</v>
+      </c>
+      <c r="E10" s="26"/>
+      <c r="F10" s="37" t="s">
+        <v>68</v>
+      </c>
+      <c r="G10" s="38" t="s">
+        <v>69</v>
+      </c>
+      <c r="H10" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="I9" s="29" t="s">
-        <v>38</v>
-      </c>
-      <c r="J9" s="11">
-        <v>1855</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" ht="34.5">
-      <c r="A10" s="11">
-        <v>174</v>
-      </c>
-      <c r="B10" s="24" t="s">
-        <v>46</v>
-      </c>
-      <c r="C10" s="11">
-        <v>14</v>
-      </c>
-      <c r="D10" s="25" t="s">
-        <v>47</v>
-      </c>
-      <c r="E10" s="26"/>
-      <c r="F10" s="27" t="s">
-        <v>48</v>
-      </c>
-      <c r="G10" s="35" t="s">
-        <v>49</v>
-      </c>
-      <c r="H10" s="2" t="s">
-        <v>51</v>
-      </c>
       <c r="I10" s="29" t="s">
-        <v>50</v>
+        <v>71</v>
       </c>
       <c r="J10" s="11">
-        <v>2183</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" ht="34.5">
+        <v>13418</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" ht="86.25">
       <c r="A11" s="11">
-        <v>120</v>
-      </c>
-      <c r="B11" s="32" t="s">
-        <v>52</v>
+        <v>85</v>
+      </c>
+      <c r="B11" s="24" t="s">
+        <v>24</v>
       </c>
       <c r="C11" s="11">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="D11" s="25" t="s">
-        <v>53</v>
-      </c>
-      <c r="E11" s="26"/>
+        <v>25</v>
+      </c>
+      <c r="E11" s="26" t="s">
+        <v>25</v>
+      </c>
       <c r="F11" s="27" t="s">
-        <v>54</v>
+        <v>26</v>
       </c>
       <c r="G11" s="28" t="s">
-        <v>55</v>
-      </c>
-      <c r="H11" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="I11" s="31" t="s">
-        <v>56</v>
-      </c>
-      <c r="J11" s="22">
-        <v>5246</v>
+        <v>27</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="I11" s="29" t="s">
+        <v>28</v>
+      </c>
+      <c r="J11" s="11">
+        <v>15129</v>
+      </c>
+      <c r="K11" s="11" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="12" spans="1:14" ht="34.5">
       <c r="A12" s="11">
-        <v>1</v>
-      </c>
-      <c r="B12" s="32" t="s">
-        <v>57</v>
+        <v>130</v>
+      </c>
+      <c r="B12" s="24" t="s">
+        <v>72</v>
       </c>
       <c r="C12" s="11">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D12" s="25" t="s">
-        <v>58</v>
+        <v>73</v>
       </c>
       <c r="E12" s="26"/>
       <c r="F12" s="27" t="s">
-        <v>59</v>
-      </c>
-      <c r="G12" s="28" t="s">
-        <v>60</v>
+        <v>74</v>
+      </c>
+      <c r="G12" s="35" t="s">
+        <v>75</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="I12" s="13" t="s">
-        <v>61</v>
-      </c>
-      <c r="J12" s="22">
-        <v>6498</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" ht="34.5">
+        <v>51</v>
+      </c>
+      <c r="I12" s="29" t="s">
+        <v>76</v>
+      </c>
+      <c r="J12" s="11">
+        <v>15606</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" ht="51.75">
       <c r="A13" s="11">
-        <v>26</v>
+        <v>9</v>
       </c>
       <c r="B13" s="24" t="s">
-        <v>62</v>
+        <v>93</v>
       </c>
       <c r="C13" s="11">
-        <v>9</v>
-      </c>
-      <c r="D13" s="25" t="s">
-        <v>63</v>
+        <v>8</v>
+      </c>
+      <c r="D13" s="32" t="s">
+        <v>94</v>
       </c>
       <c r="E13" s="26"/>
-      <c r="F13" s="36" t="s">
-        <v>64</v>
-      </c>
-      <c r="G13" s="35" t="s">
-        <v>65</v>
-      </c>
-      <c r="H13" s="2" t="s">
+      <c r="F13" s="27" t="s">
+        <v>95</v>
+      </c>
+      <c r="G13" s="39" t="s">
+        <v>96</v>
+      </c>
+      <c r="H13" s="17" t="s">
+        <v>98</v>
+      </c>
+      <c r="I13" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="J13" s="22">
+        <v>15761</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" ht="34.5">
+      <c r="A14" s="11">
+        <v>85</v>
+      </c>
+      <c r="B14" s="24" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14" s="11">
+        <v>14</v>
+      </c>
+      <c r="D14" s="25" t="s">
+        <v>77</v>
+      </c>
+      <c r="E14" s="26"/>
+      <c r="F14" s="36" t="s">
+        <v>78</v>
+      </c>
+      <c r="G14" s="35" t="s">
+        <v>79</v>
+      </c>
+      <c r="H14" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="I13" s="13" t="s">
-        <v>66</v>
-      </c>
-      <c r="J13" s="22">
-        <v>12089</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" ht="61.5">
-      <c r="A14" s="11">
-        <v>78</v>
-      </c>
-      <c r="B14" s="32" t="s">
-        <v>67</v>
-      </c>
-      <c r="C14" s="11">
-        <v>16</v>
-      </c>
-      <c r="D14" s="33" t="s">
-        <v>70</v>
-      </c>
-      <c r="E14" s="26"/>
-      <c r="F14" s="37" t="s">
-        <v>68</v>
-      </c>
-      <c r="G14" s="38" t="s">
-        <v>69</v>
-      </c>
-      <c r="H14" s="2" t="s">
-        <v>45</v>
-      </c>
       <c r="I14" s="29" t="s">
-        <v>71</v>
+        <v>80</v>
       </c>
       <c r="J14" s="11">
-        <v>13418</v>
+        <v>16145</v>
       </c>
     </row>
     <row r="15" spans="1:14" ht="34.5">
       <c r="A15" s="11">
-        <v>130</v>
+        <v>5</v>
       </c>
       <c r="B15" s="24" t="s">
-        <v>72</v>
+        <v>81</v>
       </c>
       <c r="C15" s="11">
-        <v>9</v>
-      </c>
-      <c r="D15" s="25" t="s">
-        <v>73</v>
+        <v>18</v>
+      </c>
+      <c r="D15" s="32" t="s">
+        <v>82</v>
       </c>
       <c r="E15" s="26"/>
       <c r="F15" s="27" t="s">
-        <v>74</v>
-      </c>
-      <c r="G15" s="35" t="s">
-        <v>75</v>
-      </c>
-      <c r="H15" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="I15" s="29" t="s">
-        <v>76</v>
+        <v>83</v>
+      </c>
+      <c r="G15" s="39" t="s">
+        <v>84</v>
+      </c>
+      <c r="H15" s="17" t="s">
+        <v>85</v>
+      </c>
+      <c r="I15" s="40" t="s">
+        <v>86</v>
       </c>
       <c r="J15" s="11">
-        <v>15606</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" ht="34.5">
+        <v>16517</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" ht="61.5">
       <c r="A16" s="11">
+        <v>109</v>
+      </c>
+      <c r="B16" s="24" t="s">
+        <v>87</v>
+      </c>
+      <c r="C16" s="11">
+        <v>12</v>
+      </c>
+      <c r="D16" s="32" t="s">
+        <v>88</v>
+      </c>
+      <c r="E16" s="20" t="s">
+        <v>89</v>
+      </c>
+      <c r="F16" s="27" t="s">
+        <v>90</v>
+      </c>
+      <c r="G16" s="28" t="s">
+        <v>91</v>
+      </c>
+      <c r="H16" s="17" t="s">
         <v>85</v>
       </c>
-      <c r="B16" s="24" t="s">
-        <v>24</v>
-      </c>
-      <c r="C16" s="11">
-        <v>14</v>
-      </c>
-      <c r="D16" s="25" t="s">
-        <v>77</v>
-      </c>
-      <c r="E16" s="26"/>
-      <c r="F16" s="36" t="s">
-        <v>78</v>
-      </c>
-      <c r="G16" s="35" t="s">
-        <v>79</v>
-      </c>
-      <c r="H16" s="17" t="s">
-        <v>51</v>
-      </c>
-      <c r="I16" s="29" t="s">
-        <v>80</v>
-      </c>
-      <c r="J16" s="11">
-        <v>16145</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" ht="34.5">
-      <c r="A17" s="11">
-        <v>5</v>
-      </c>
-      <c r="B17" s="24" t="s">
-        <v>81</v>
-      </c>
-      <c r="C17" s="11">
+      <c r="I16" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="J16" s="22">
+        <v>16615</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10">
+      <c r="B17" s="24"/>
+      <c r="F17" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="H17" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="I17" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="J17" s="5">
+        <v>90001</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="34.5">
+      <c r="B18" s="24"/>
+      <c r="C18" s="23"/>
+      <c r="F18" s="15" t="s">
+        <v>102</v>
+      </c>
+      <c r="H18" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="I18" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="J18" s="5">
+        <v>90002</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10">
+      <c r="B19" s="24"/>
+      <c r="C19" s="23"/>
+      <c r="E19" s="20"/>
+      <c r="F19" s="15" t="s">
+        <v>103</v>
+      </c>
+      <c r="H19" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="I19" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="J19" s="5">
+        <v>90003</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" ht="69">
+      <c r="A20" s="22">
+        <v>121</v>
+      </c>
+      <c r="B20" s="24" t="s">
+        <v>104</v>
+      </c>
+      <c r="C20" s="22">
         <v>18</v>
       </c>
-      <c r="D17" s="32" t="s">
-        <v>82</v>
-      </c>
-      <c r="E17" s="26"/>
-      <c r="F17" s="27" t="s">
-        <v>83</v>
-      </c>
-      <c r="G17" s="39" t="s">
-        <v>84</v>
-      </c>
-      <c r="H17" s="17" t="s">
-        <v>85</v>
-      </c>
-      <c r="I17" s="40" t="s">
-        <v>86</v>
-      </c>
-      <c r="J17" s="11">
-        <v>16517</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" ht="61.5">
-      <c r="A18" s="11">
+      <c r="D20" s="25" t="s">
+        <v>99</v>
+      </c>
+      <c r="F20" s="15" t="s">
+        <v>101</v>
+      </c>
+      <c r="G20" s="16" t="s">
+        <v>116</v>
+      </c>
+      <c r="H20" s="17" t="s">
+        <v>120</v>
+      </c>
+      <c r="I20" s="13" t="s">
+        <v>100</v>
+      </c>
+      <c r="J20" s="5">
+        <v>90004</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" ht="69">
+      <c r="A21" s="22">
+        <v>32</v>
+      </c>
+      <c r="B21" s="22" t="s">
+        <v>108</v>
+      </c>
+      <c r="C21" s="41">
+        <v>17</v>
+      </c>
+      <c r="D21" s="25" t="s">
+        <v>107</v>
+      </c>
+      <c r="F21" s="15" t="s">
+        <v>113</v>
+      </c>
+      <c r="G21" s="16" t="s">
+        <v>114</v>
+      </c>
+      <c r="H21" s="17" t="s">
+        <v>117</v>
+      </c>
+      <c r="I21" s="13" t="s">
+        <v>115</v>
+      </c>
+      <c r="J21" s="5">
+        <v>90005</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" ht="86.25">
+      <c r="A22" s="22">
+        <v>121</v>
+      </c>
+      <c r="B22" s="24" t="s">
+        <v>104</v>
+      </c>
+      <c r="C22" s="22">
+        <v>18</v>
+      </c>
+      <c r="D22" s="25" t="s">
+        <v>99</v>
+      </c>
+      <c r="F22" s="15" t="s">
         <v>109</v>
       </c>
-      <c r="B18" s="24" t="s">
-        <v>87</v>
-      </c>
-      <c r="C18" s="11">
-        <v>12</v>
-      </c>
-      <c r="D18" s="32" t="s">
-        <v>88</v>
-      </c>
-      <c r="E18" s="20" t="s">
-        <v>89</v>
-      </c>
-      <c r="F18" s="27" t="s">
-        <v>90</v>
-      </c>
-      <c r="G18" s="28" t="s">
-        <v>91</v>
-      </c>
-      <c r="H18" s="17" t="s">
-        <v>85</v>
-      </c>
-      <c r="I18" s="13" t="s">
-        <v>92</v>
-      </c>
-      <c r="J18" s="22">
-        <v>16615</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" ht="51.75">
-      <c r="A19" s="11">
-        <v>9</v>
-      </c>
-      <c r="B19" s="24" t="s">
-        <v>93</v>
-      </c>
-      <c r="C19" s="11">
-        <v>8</v>
-      </c>
-      <c r="D19" s="32" t="s">
-        <v>94</v>
-      </c>
-      <c r="E19" s="26"/>
-      <c r="F19" s="27" t="s">
-        <v>95</v>
-      </c>
-      <c r="G19" s="39" t="s">
-        <v>96</v>
-      </c>
-      <c r="H19" s="17" t="s">
-        <v>98</v>
-      </c>
-      <c r="I19" s="13" t="s">
-        <v>97</v>
-      </c>
-      <c r="J19" s="22">
-        <v>15761</v>
+      <c r="G22" s="16" t="s">
+        <v>105</v>
+      </c>
+      <c r="H22" s="17" t="s">
+        <v>118</v>
+      </c>
+      <c r="I22" s="13" t="s">
+        <v>110</v>
+      </c>
+      <c r="J22" s="5">
+        <v>90006</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" ht="86.25">
+      <c r="A23" s="22">
+        <v>121</v>
+      </c>
+      <c r="B23" s="24" t="s">
+        <v>104</v>
+      </c>
+      <c r="C23" s="22">
+        <v>18</v>
+      </c>
+      <c r="D23" s="25" t="s">
+        <v>99</v>
+      </c>
+      <c r="F23" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="G23" s="16" t="s">
+        <v>106</v>
+      </c>
+      <c r="H23" s="17" t="s">
+        <v>119</v>
+      </c>
+      <c r="I23" s="13" t="s">
+        <v>112</v>
+      </c>
+      <c r="J23" s="5">
+        <v>90007</v>
       </c>
     </row>
   </sheetData>
+  <sortState ref="A21:J23">
+    <sortCondition ref="F21:F23"/>
+  </sortState>
   <hyperlinks>
-    <hyperlink ref="B7" r:id="rId1" display="https://www.zdic.net/zd/bs/?bs=%E5%B7%BE"/>
-    <hyperlink ref="B8" r:id="rId2" display="https://www.zdic.net/zd/bs/?bs=%E6%94%B4"/>
-    <hyperlink ref="B9" r:id="rId3" display="https://www.zdic.net/zd/bs/?bs=%E6%94%B4"/>
-    <hyperlink ref="G10" r:id="rId4" tooltip="jìng" display="https://en.wiktionary.org/wiki/j%C3%ACng"/>
-    <hyperlink ref="B11" r:id="rId5" display="https://www.zdic.net/zd/bs/?bs=%E7%B3%B8"/>
-    <hyperlink ref="B12" r:id="rId6" display="https://www.zdic.net/zd/bs/?bs=%E4%B8%80"/>
-    <hyperlink ref="G13" r:id="rId7" tooltip="ruǎn" display="https://en.wiktionary.org/wiki/ru%C7%8En"/>
-    <hyperlink ref="B14" r:id="rId8" display="https://www.zdic.net/zd/bs/?bs=%E6%AD%B9"/>
-    <hyperlink ref="G15" r:id="rId9" tooltip="xīng" display="https://en.wiktionary.org/wiki/x%C4%ABng"/>
-    <hyperlink ref="G16" r:id="rId10" tooltip="sǒng" display="https://en.wiktionary.org/wiki/s%C7%92ng"/>
-    <hyperlink ref="D17" r:id="rId11" display="https://www.zdic.net/hans/%E6%AA%BF"/>
-    <hyperlink ref="D18" r:id="rId12" location="Chinese" tooltip="睍" display="https://en.wiktionary.org/wiki/%E7%9D%8D - Chinese"/>
-    <hyperlink ref="D19" r:id="rId13" display="http://humanum.arts.cuhk.edu.hk/Lexis/lexi-can/search.php?q=%CB%C2"/>
+    <hyperlink ref="B2" r:id="rId1" display="https://www.zdic.net/zd/bs/?bs=%E5%B7%BE"/>
+    <hyperlink ref="B3" r:id="rId2" display="https://www.zdic.net/zd/bs/?bs=%E6%94%B4"/>
+    <hyperlink ref="B4" r:id="rId3" display="https://www.zdic.net/zd/bs/?bs=%E6%94%B4"/>
+    <hyperlink ref="G5" r:id="rId4" tooltip="jìng" display="https://en.wiktionary.org/wiki/j%C3%ACng"/>
+    <hyperlink ref="B7" r:id="rId5" display="https://www.zdic.net/zd/bs/?bs=%E7%B3%B8"/>
+    <hyperlink ref="B8" r:id="rId6" display="https://www.zdic.net/zd/bs/?bs=%E4%B8%80"/>
+    <hyperlink ref="G9" r:id="rId7" tooltip="ruǎn" display="https://en.wiktionary.org/wiki/ru%C7%8En"/>
+    <hyperlink ref="B10" r:id="rId8" display="https://www.zdic.net/zd/bs/?bs=%E6%AD%B9"/>
+    <hyperlink ref="G12" r:id="rId9" tooltip="xīng" display="https://en.wiktionary.org/wiki/x%C4%ABng"/>
+    <hyperlink ref="G14" r:id="rId10" tooltip="sǒng" display="https://en.wiktionary.org/wiki/s%C7%92ng"/>
+    <hyperlink ref="D15" r:id="rId11" display="https://www.zdic.net/hans/%E6%AA%BF"/>
+    <hyperlink ref="D16" r:id="rId12" location="Chinese" tooltip="睍" display="https://en.wiktionary.org/wiki/%E7%9D%8D - Chinese"/>
+    <hyperlink ref="D13" r:id="rId13" display="http://humanum.arts.cuhk.edu.hk/Lexis/lexi-can/search.php?q=%CB%C2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId14"/>

</xml_diff>

<commit_message>
added IDC to hel5 ⿰缶堯 and pit2 ⿰匹毛
</commit_message>
<xml_diff>
--- a/hed/addenda/addendum.xlsx
+++ b/hed/addenda/addendum.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="10245" yWindow="-300" windowWidth="22350" windowHeight="12600" tabRatio="405"/>
+    <workbookView xWindow="14280" yWindow="-300" windowWidth="18315" windowHeight="12600" tabRatio="405"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="121">
   <si>
     <t>pit2</t>
   </si>
@@ -230,41 +230,12 @@
     <t>缶</t>
   </si>
   <si>
-    <t xml:space="preserve">𦉗 </t>
-  </si>
-  <si>
     <t>hêl</t>
   </si>
   <si>
     <t>tiào</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">&lt;台&gt; 𦉗 hêl a large clay cooking pot.¹²¹ʼ⁰
-(composition: ⿰缶堯; U+26257).
-&lt;又&gt; não, yẽl. </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Segoe UI"/>
-        <family val="2"/>
-      </rPr>
-      <t>(See 𦉗 não, 𦉗 yẽl.)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Segoe UI"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-  </si>
-  <si>
     <t>hel5</t>
   </si>
   <si>
@@ -280,51 +251,6 @@
     <t>liáo</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Vietnamese pronunciation </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Segoe UI"/>
-        <family val="2"/>
-      </rPr>
-      <t>niêu</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Segoe UI"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">: a small casserole.¹¹³
-(composition: ⿰土僚; U+214AD).
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Segoe UI"/>
-        <family val="2"/>
-      </rPr>
-      <t>(See 𦉗 não, 𦉗 yẽl.)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Segoe UI"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-  </si>
-  <si>
     <t>lel3</t>
   </si>
   <si>
@@ -334,51 +260,6 @@
     <t>náo</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">found in Taiwanese names. Same as Vietnamese 𡒭 </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Segoe UI"/>
-        <family val="2"/>
-      </rPr>
-      <t>niêu</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Segoe UI"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">: a small casserole.¹¹³
-(composition: ⿰缶堯; U+26257).
-&lt;又&gt; hêl, yẽl. </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Segoe UI"/>
-        <family val="2"/>
-      </rPr>
-      <t>(See 𦉗 hêl, 𡒭 lẽl, 𦉗 yẽl.)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Segoe UI"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-  </si>
-  <si>
     <t>nao3</t>
   </si>
   <si>
@@ -386,32 +267,6 @@
   </si>
   <si>
     <t>yáo</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">found in Taiwanese names. Same as Vietnamese 𡒭 niêu: a small casserole.¹¹³
-(composition: ⿰缶堯; U+26257).
-&lt;又&gt; hêl, não. </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Segoe UI"/>
-        <family val="2"/>
-      </rPr>
-      <t>(See 𦉗 hêl, 𡒭 lẽl, 𦉗 não.)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Segoe UI"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
   </si>
   <si>
     <t>yel3</t>
@@ -856,95 +711,7 @@
     <t>pī</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">&lt;台&gt; 𣬮 pït loose (such as a knot becoming loose). 
-cf 松[鬆] xüng </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Segoe UI"/>
-        <family val="2"/>
-      </rPr>
-      <t>sōng</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Segoe UI"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> loose; to loosen.
-(composition ⿰匹毛; U+23B2E).
-&lt;又&gt; bì. </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Segoe UI"/>
-        <family val="2"/>
-      </rPr>
-      <t>(See 𣬮 bì).</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Segoe UI"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-  </si>
-  <si>
     <t>bì</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">same as 髲 bì </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <rFont val="Segoe UI"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">bì </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Segoe UI"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">a wig.⁸
-(composition ⿰匹毛; U+23B2E).
-&lt;又&gt; pït. </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Segoe UI"/>
-        <family val="2"/>
-      </rPr>
-      <t>(See 𣬮 pït; 髲 bì).</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Segoe UI"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
   </si>
   <si>
     <t>bi4</t>
@@ -1450,12 +1217,470 @@
   <si>
     <t>ngeik1</t>
   </si>
+  <si>
+    <r>
+      <t>&lt;台&gt; 𣬮</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="0" tint="-0.34998626667073579"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">❄{⿰匹毛} </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">pït loose (such as a knot becoming loose). 
+cf 松[鬆] xüng </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t>sōng</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> loose; to loosen.
+(composition ⿰匹毛; U+23B2E).
+&lt;又&gt; bì. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">(See </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t>𣬮</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="0" tint="-0.34998626667073579"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t>❄{⿰匹毛}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> bì).</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">same as 髲 bì </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">bì </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">a wig.⁸
+(composition ⿰匹毛; U+23B2E).
+&lt;又&gt; pït. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t>(See 𣬮</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="0" tint="-0.34998626667073579"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t>❄{⿰匹毛}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> pït; 髲 bì).</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">𦉗
+❄ </t>
+  </si>
+  <si>
+    <r>
+      <t>&lt;台&gt; 𦉗</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="0" tint="-0.34998626667073579"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t>❄{⿰缶堯}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> hêl a large clay cooking pot.¹²¹ʼ⁰
+(composition: ⿰缶堯; U+26257).
+&lt;又&gt; não, yẽl. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t>(See 𦉗</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="0" tint="-0.34998626667073579"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t>❄{⿰缶堯}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> não, 𦉗</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="0" tint="-0.34998626667073579"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t>❄{⿰缶堯</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t>} yẽl.)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Vietnamese pronunciation </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t>niêu</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">: a small casserole.¹¹³
+(composition: ⿰土僚; U+214AD).
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t>(See 𦉗</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="0" tint="-0.34998626667073579"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t>❄{⿰缶堯}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> não, 𦉗</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="0" tint="-0.34998626667073579"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t>❄{⿰缶堯}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> yẽl.)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">found in Taiwanese names. Same as Vietnamese 𡒭 </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t>niêu</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">: a small casserole.¹¹³
+(composition: ⿰缶堯; U+26257).
+&lt;又&gt; hêl, yẽl. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t>(See 𦉗</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="0" tint="-0.34998626667073579"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t>❄{⿰缶堯}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> hêl, 𡒭 lẽl, 𦉗</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="0" tint="-0.34998626667073579"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t>❄{⿰缶堯}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> yẽl.)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">found in Taiwanese names. Same as Vietnamese 𡒭 niêu: a small casserole.¹¹³
+(composition: ⿰缶堯; U+26257).
+&lt;又&gt; hêl, não. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t>(See 𦉗</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="0" tint="-0.34998626667073579"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t>❄{⿰缶堯}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> hêl, 𡒭 lẽl, 𦉗</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="0" tint="-0.34998626667073579"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t>❄{⿰缶堯}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> não.)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="27">
+  <fonts count="28">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1616,6 +1841,12 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <color theme="0" tint="-0.34998626667073579"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1638,7 +1869,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1699,9 +1930,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -1739,31 +1967,31 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2063,7 +2291,7 @@
   <dimension ref="A1:N24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="K23" sqref="A1:K23"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30.75"/>
@@ -2071,7 +2299,7 @@
     <col min="1" max="1" width="3.5703125" style="19" customWidth="1"/>
     <col min="2" max="2" width="2.85546875" style="19" customWidth="1"/>
     <col min="3" max="3" width="2.7109375" style="19" customWidth="1"/>
-    <col min="4" max="4" width="6.42578125" style="35" customWidth="1"/>
+    <col min="4" max="4" width="6.42578125" style="34" customWidth="1"/>
     <col min="5" max="5" width="5.42578125" style="17" customWidth="1"/>
     <col min="6" max="6" width="9.140625" style="13" customWidth="1"/>
     <col min="7" max="7" width="11.28515625" style="14" customWidth="1"/>
@@ -2095,7 +2323,7 @@
       <c r="C1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="41" t="s">
+      <c r="D1" s="38" t="s">
         <v>5</v>
       </c>
       <c r="E1" s="5" t="s">
@@ -2130,7 +2358,7 @@
       <c r="C2" s="19">
         <v>12</v>
       </c>
-      <c r="D2" s="36" t="s">
+      <c r="D2" s="34" t="s">
         <v>16</v>
       </c>
       <c r="F2" s="12" t="s">
@@ -2163,7 +2391,7 @@
       <c r="C3" s="19">
         <v>12</v>
       </c>
-      <c r="D3" s="36" t="s">
+      <c r="D3" s="34" t="s">
         <v>16</v>
       </c>
       <c r="F3" s="12" t="s">
@@ -2196,7 +2424,7 @@
       <c r="C4" s="19">
         <v>12</v>
       </c>
-      <c r="D4" s="36" t="s">
+      <c r="D4" s="34" t="s">
         <v>16</v>
       </c>
       <c r="F4" s="12" t="s">
@@ -2226,7 +2454,7 @@
       <c r="C5" s="19">
         <v>12</v>
       </c>
-      <c r="D5" s="36" t="s">
+      <c r="D5" s="34" t="s">
         <v>16</v>
       </c>
       <c r="F5" s="12" t="s">
@@ -2256,20 +2484,20 @@
       <c r="C6" s="19">
         <v>18</v>
       </c>
-      <c r="D6" s="37" t="s">
+      <c r="D6" s="41" t="s">
+        <v>116</v>
+      </c>
+      <c r="F6" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="F6" s="13" t="s">
+      <c r="G6" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="G6" s="14" t="s">
+      <c r="H6" s="15" t="s">
+        <v>117</v>
+      </c>
+      <c r="I6" s="11" t="s">
         <v>36</v>
-      </c>
-      <c r="H6" s="15" t="s">
-        <v>37</v>
-      </c>
-      <c r="I6" s="11" t="s">
-        <v>38</v>
       </c>
       <c r="J6" s="4">
         <v>90005</v>
@@ -2281,25 +2509,25 @@
         <v>32</v>
       </c>
       <c r="B7" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="C7" s="22">
+        <v>17</v>
+      </c>
+      <c r="D7" s="42" t="s">
+        <v>38</v>
+      </c>
+      <c r="F7" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="C7" s="23">
-        <v>17</v>
-      </c>
-      <c r="D7" s="37" t="s">
+      <c r="G7" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="F7" s="13" t="s">
+      <c r="H7" s="15" t="s">
+        <v>118</v>
+      </c>
+      <c r="I7" s="11" t="s">
         <v>41</v>
-      </c>
-      <c r="G7" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="H7" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="I7" s="11" t="s">
-        <v>44</v>
       </c>
       <c r="J7" s="4">
         <v>90006</v>
@@ -2316,20 +2544,20 @@
       <c r="C8" s="19">
         <v>18</v>
       </c>
-      <c r="D8" s="37" t="s">
-        <v>34</v>
+      <c r="D8" s="41" t="s">
+        <v>116</v>
       </c>
       <c r="F8" s="13" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="G8" s="14" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="H8" s="15" t="s">
-        <v>47</v>
+        <v>119</v>
       </c>
       <c r="I8" s="11" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="J8" s="4">
         <v>90007</v>
@@ -2346,20 +2574,20 @@
       <c r="C9" s="19">
         <v>18</v>
       </c>
-      <c r="D9" s="37" t="s">
-        <v>34</v>
+      <c r="D9" s="41" t="s">
+        <v>116</v>
       </c>
       <c r="F9" s="13" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="G9" s="14" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="H9" s="15" t="s">
-        <v>51</v>
+        <v>120</v>
       </c>
       <c r="I9" s="11" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="J9" s="4">
         <v>90008</v>
@@ -2370,29 +2598,29 @@
       <c r="A10" s="2">
         <v>167</v>
       </c>
-      <c r="B10" s="24" t="s">
-        <v>53</v>
+      <c r="B10" s="23" t="s">
+        <v>48</v>
       </c>
       <c r="C10" s="2">
         <v>14</v>
       </c>
-      <c r="D10" s="38" t="s">
+      <c r="D10" s="35" t="s">
+        <v>49</v>
+      </c>
+      <c r="E10" s="24" t="s">
+        <v>50</v>
+      </c>
+      <c r="F10" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="G10" s="26" t="s">
+        <v>52</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="I10" s="27" t="s">
         <v>54</v>
-      </c>
-      <c r="E10" s="25" t="s">
-        <v>55</v>
-      </c>
-      <c r="F10" s="26" t="s">
-        <v>56</v>
-      </c>
-      <c r="G10" s="27" t="s">
-        <v>57</v>
-      </c>
-      <c r="H10" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="I10" s="28" t="s">
-        <v>59</v>
       </c>
       <c r="J10" s="4">
         <v>90009</v>
@@ -2403,29 +2631,29 @@
       <c r="A11" s="2">
         <v>167</v>
       </c>
-      <c r="B11" s="24" t="s">
-        <v>53</v>
+      <c r="B11" s="23" t="s">
+        <v>48</v>
       </c>
       <c r="C11" s="2">
         <v>14</v>
       </c>
-      <c r="D11" s="38" t="s">
-        <v>54</v>
-      </c>
-      <c r="E11" s="25" t="s">
+      <c r="D11" s="35" t="s">
+        <v>49</v>
+      </c>
+      <c r="E11" s="24" t="s">
+        <v>50</v>
+      </c>
+      <c r="F11" s="25" t="s">
         <v>55</v>
       </c>
-      <c r="F11" s="26" t="s">
-        <v>60</v>
-      </c>
-      <c r="G11" s="27" t="s">
-        <v>61</v>
+      <c r="G11" s="26" t="s">
+        <v>56</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="I11" s="28" t="s">
-        <v>63</v>
+        <v>57</v>
+      </c>
+      <c r="I11" s="27" t="s">
+        <v>58</v>
       </c>
       <c r="J11" s="4">
         <v>90010</v>
@@ -2436,29 +2664,29 @@
       <c r="A12" s="2">
         <v>167</v>
       </c>
-      <c r="B12" s="24" t="s">
-        <v>53</v>
+      <c r="B12" s="23" t="s">
+        <v>48</v>
       </c>
       <c r="C12" s="2">
         <v>14</v>
       </c>
-      <c r="D12" s="38" t="s">
-        <v>54</v>
-      </c>
-      <c r="E12" s="25" t="s">
-        <v>55</v>
-      </c>
-      <c r="F12" s="26" t="s">
-        <v>64</v>
-      </c>
-      <c r="G12" s="27" t="s">
+      <c r="D12" s="35" t="s">
+        <v>49</v>
+      </c>
+      <c r="E12" s="24" t="s">
+        <v>50</v>
+      </c>
+      <c r="F12" s="25" t="s">
+        <v>59</v>
+      </c>
+      <c r="G12" s="26" t="s">
+        <v>56</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="I12" s="27" t="s">
         <v>61</v>
-      </c>
-      <c r="H12" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="I12" s="28" t="s">
-        <v>66</v>
       </c>
       <c r="J12" s="4">
         <v>90011</v>
@@ -2469,27 +2697,27 @@
       <c r="A13" s="2">
         <v>38</v>
       </c>
-      <c r="B13" s="29" t="s">
+      <c r="B13" s="28" t="s">
+        <v>62</v>
+      </c>
+      <c r="C13" s="29">
+        <v>7</v>
+      </c>
+      <c r="D13" s="35" t="s">
+        <v>63</v>
+      </c>
+      <c r="E13" s="30"/>
+      <c r="F13" s="31" t="s">
+        <v>64</v>
+      </c>
+      <c r="G13" s="32" t="s">
+        <v>65</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="I13" s="27" t="s">
         <v>67</v>
-      </c>
-      <c r="C13" s="30">
-        <v>7</v>
-      </c>
-      <c r="D13" s="38" t="s">
-        <v>68</v>
-      </c>
-      <c r="E13" s="31"/>
-      <c r="F13" s="32" t="s">
-        <v>69</v>
-      </c>
-      <c r="G13" s="33" t="s">
-        <v>70</v>
-      </c>
-      <c r="H13" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="I13" s="28" t="s">
-        <v>72</v>
       </c>
       <c r="J13" s="4">
         <v>90012</v>
@@ -2500,29 +2728,29 @@
       <c r="A14" s="2">
         <v>159</v>
       </c>
-      <c r="B14" s="24" t="s">
-        <v>73</v>
+      <c r="B14" s="23" t="s">
+        <v>68</v>
       </c>
       <c r="C14" s="2">
         <v>13</v>
       </c>
-      <c r="D14" s="38" t="s">
-        <v>74</v>
-      </c>
-      <c r="E14" s="25" t="s">
-        <v>75</v>
-      </c>
-      <c r="F14" s="26" t="s">
-        <v>76</v>
-      </c>
-      <c r="G14" s="27" t="s">
-        <v>77</v>
+      <c r="D14" s="35" t="s">
+        <v>69</v>
+      </c>
+      <c r="E14" s="24" t="s">
+        <v>70</v>
+      </c>
+      <c r="F14" s="25" t="s">
+        <v>71</v>
+      </c>
+      <c r="G14" s="26" t="s">
+        <v>72</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="I14" s="28" t="s">
-        <v>78</v>
+        <v>99</v>
+      </c>
+      <c r="I14" s="27" t="s">
+        <v>73</v>
       </c>
       <c r="J14" s="4">
         <v>90013</v>
@@ -2533,62 +2761,62 @@
       <c r="A15" s="2">
         <v>30</v>
       </c>
-      <c r="B15" s="24" t="s">
+      <c r="B15" s="23" t="s">
         <v>15</v>
       </c>
       <c r="C15" s="2">
         <v>13</v>
       </c>
-      <c r="D15" s="36" t="s">
-        <v>79</v>
+      <c r="D15" s="34" t="s">
+        <v>74</v>
       </c>
       <c r="E15" s="17" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="F15" s="13" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="G15" s="14" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="H15" s="15" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="I15" s="11" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="J15" s="4">
         <v>90014</v>
       </c>
       <c r="K15"/>
     </row>
-    <row r="16" spans="1:14" ht="155.25">
+    <row r="16" spans="1:14" ht="138">
       <c r="A16" s="2">
         <v>64</v>
       </c>
-      <c r="B16" s="24" t="s">
-        <v>84</v>
+      <c r="B16" s="23" t="s">
+        <v>79</v>
       </c>
       <c r="C16" s="2">
         <v>20</v>
       </c>
-      <c r="D16" s="38" t="s">
-        <v>85</v>
-      </c>
-      <c r="E16" s="25" t="s">
-        <v>86</v>
-      </c>
-      <c r="F16" s="26" t="s">
-        <v>87</v>
-      </c>
-      <c r="G16" s="33" t="s">
-        <v>88</v>
+      <c r="D16" s="35" t="s">
+        <v>80</v>
+      </c>
+      <c r="E16" s="24" t="s">
+        <v>81</v>
+      </c>
+      <c r="F16" s="25" t="s">
+        <v>82</v>
+      </c>
+      <c r="G16" s="32" t="s">
+        <v>83</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="I16" s="34" t="s">
-        <v>89</v>
+        <v>101</v>
+      </c>
+      <c r="I16" s="33" t="s">
+        <v>84</v>
       </c>
       <c r="J16" s="4">
         <v>90015</v>
@@ -2600,22 +2828,22 @@
         <v>82</v>
       </c>
       <c r="B17" s="21" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="C17" s="20">
         <v>8</v>
       </c>
-      <c r="D17" s="39" t="s">
-        <v>91</v>
+      <c r="D17" s="36" t="s">
+        <v>86</v>
       </c>
       <c r="F17" s="13" t="s">
         <v>13</v>
       </c>
       <c r="G17" s="14" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="H17" s="15" t="s">
-        <v>93</v>
+        <v>114</v>
       </c>
       <c r="I17" s="11" t="s">
         <v>0</v>
@@ -2630,26 +2858,26 @@
         <v>190</v>
       </c>
       <c r="B18" s="21" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="C18" s="20">
         <v>8</v>
       </c>
-      <c r="D18" s="40" t="s">
-        <v>91</v>
-      </c>
-      <c r="E18" s="25"/>
-      <c r="F18" s="32" t="s">
-        <v>94</v>
-      </c>
-      <c r="G18" s="33" t="s">
-        <v>94</v>
+      <c r="D18" s="37" t="s">
+        <v>86</v>
+      </c>
+      <c r="E18" s="24"/>
+      <c r="F18" s="31" t="s">
+        <v>88</v>
+      </c>
+      <c r="G18" s="32" t="s">
+        <v>88</v>
       </c>
       <c r="H18" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="I18" s="28" t="s">
-        <v>96</v>
+        <v>115</v>
+      </c>
+      <c r="I18" s="27" t="s">
+        <v>89</v>
       </c>
       <c r="J18" s="4">
         <v>90017</v>
@@ -2660,24 +2888,24 @@
       <c r="A19" s="2">
         <v>30</v>
       </c>
-      <c r="B19" s="24" t="s">
+      <c r="B19" s="23" t="s">
         <v>15</v>
       </c>
       <c r="C19" s="2">
         <v>13</v>
       </c>
-      <c r="D19" s="38" t="s">
-        <v>97</v>
+      <c r="D19" s="35" t="s">
+        <v>90</v>
       </c>
       <c r="E19" s="18"/>
       <c r="F19" s="13" t="s">
         <v>14</v>
       </c>
       <c r="G19" s="14" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="H19" s="15" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="I19" s="11" t="s">
         <v>1</v>
@@ -2687,133 +2915,116 @@
       </c>
       <c r="K19"/>
     </row>
-    <row r="20" spans="1:11" ht="155.25">
+    <row r="20" spans="1:11" ht="138">
       <c r="A20" s="2">
         <v>86</v>
       </c>
-      <c r="B20" s="24" t="s">
-        <v>100</v>
+      <c r="B20" s="23" t="s">
+        <v>93</v>
       </c>
       <c r="C20" s="2">
         <v>14</v>
       </c>
-      <c r="D20" s="38" t="s">
-        <v>101</v>
-      </c>
-      <c r="E20" s="25"/>
-      <c r="F20" s="32" t="s">
-        <v>102</v>
+      <c r="D20" s="35" t="s">
+        <v>94</v>
+      </c>
+      <c r="E20" s="24"/>
+      <c r="F20" s="31" t="s">
+        <v>95</v>
       </c>
       <c r="G20" s="14" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="H20" s="15" t="s">
-        <v>104</v>
-      </c>
-      <c r="I20" s="28" t="s">
-        <v>105</v>
+        <v>97</v>
+      </c>
+      <c r="I20" s="27" t="s">
+        <v>98</v>
       </c>
       <c r="J20" s="4">
         <v>90019</v>
       </c>
       <c r="K20"/>
     </row>
-    <row r="21" spans="1:11" ht="155.25">
+    <row r="21" spans="1:11" ht="86.25">
       <c r="A21" s="2">
-        <v>86</v>
-      </c>
-      <c r="B21" s="24" t="s">
-        <v>100</v>
+        <v>85</v>
+      </c>
+      <c r="B21" s="23" t="s">
+        <v>102</v>
       </c>
       <c r="C21" s="2">
-        <v>14</v>
-      </c>
-      <c r="D21" s="38" t="s">
-        <v>101</v>
-      </c>
-      <c r="E21" s="25"/>
-      <c r="F21" s="32" t="s">
-        <v>102</v>
-      </c>
-      <c r="G21" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="D21" s="35" t="s">
         <v>103</v>
       </c>
-      <c r="H21" s="15" t="s">
+      <c r="E21" s="35"/>
+      <c r="F21" s="31" t="s">
         <v>104</v>
       </c>
-      <c r="I21" s="28" t="s">
+      <c r="G21" s="32" t="s">
         <v>105</v>
       </c>
+      <c r="H21" s="39" t="s">
+        <v>107</v>
+      </c>
+      <c r="I21" s="40" t="s">
+        <v>106</v>
+      </c>
       <c r="J21" s="4">
-        <v>90019</v>
+        <v>90020</v>
       </c>
       <c r="K21"/>
     </row>
-    <row r="22" spans="1:11" ht="86.25">
+    <row r="22" spans="1:11" ht="103.5">
       <c r="A22" s="2">
-        <v>85</v>
-      </c>
-      <c r="B22" s="24" t="s">
+        <v>86</v>
+      </c>
+      <c r="B22" s="23" t="s">
+        <v>93</v>
+      </c>
+      <c r="C22" s="2">
+        <v>15</v>
+      </c>
+      <c r="D22" s="35" t="s">
+        <v>108</v>
+      </c>
+      <c r="E22" s="24" t="s">
         <v>109</v>
       </c>
-      <c r="C22" s="2">
-        <v>22</v>
-      </c>
-      <c r="D22" s="38" t="s">
+      <c r="F22" s="31" t="s">
         <v>110</v>
       </c>
-      <c r="E22" s="38"/>
-      <c r="F22" s="32" t="s">
+      <c r="G22" s="32" t="s">
         <v>111</v>
       </c>
-      <c r="G22" s="33" t="s">
+      <c r="H22" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="H22" s="42" t="s">
-        <v>114</v>
-      </c>
-      <c r="I22" s="43" t="s">
+      <c r="I22" s="27" t="s">
         <v>113</v>
       </c>
       <c r="J22" s="4">
-        <v>90020</v>
-      </c>
+        <v>90021</v>
+      </c>
+      <c r="K22"/>
     </row>
-    <row r="23" spans="1:11" ht="103.5">
-      <c r="A23" s="2">
-        <v>86</v>
-      </c>
-      <c r="B23" s="24" t="s">
-        <v>100</v>
-      </c>
-      <c r="C23" s="2">
-        <v>15</v>
-      </c>
-      <c r="D23" s="38" t="s">
-        <v>115</v>
-      </c>
-      <c r="E23" s="25" t="s">
-        <v>116</v>
-      </c>
-      <c r="F23" s="32" t="s">
-        <v>117</v>
-      </c>
-      <c r="G23" s="33" t="s">
-        <v>118</v>
-      </c>
-      <c r="H23" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="I23" s="28" t="s">
-        <v>120</v>
-      </c>
-      <c r="J23" s="4">
-        <v>90021</v>
-      </c>
+    <row r="23" spans="1:11">
+      <c r="A23" s="2"/>
+      <c r="B23" s="23"/>
+      <c r="C23" s="2"/>
+      <c r="D23" s="35"/>
+      <c r="E23" s="24"/>
+      <c r="F23" s="31"/>
+      <c r="G23" s="32"/>
+      <c r="H23" s="3"/>
+      <c r="I23" s="27"/>
+      <c r="J23" s="4"/>
     </row>
     <row r="24" spans="1:11">
       <c r="B24" s="21"/>
-      <c r="D24" s="22"/>
+      <c r="D24" s="42"/>
       <c r="H24" s="15"/>
       <c r="J24" s="4"/>
     </row>

</xml_diff>

<commit_message>
added another char to addendum
</commit_message>
<xml_diff>
--- a/hed/addenda/addendum.xlsx
+++ b/hed/addenda/addendum.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="131">
   <si>
     <t>pit2</t>
   </si>
@@ -1673,6 +1673,203 @@
       </rPr>
       <t xml:space="preserve">
 </t>
+    </r>
+  </si>
+  <si>
+    <t>木</t>
+  </si>
+  <si>
+    <t>樘</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hõng </t>
+  </si>
+  <si>
+    <t>táng</t>
+  </si>
+  <si>
+    <t>sẽin</t>
+  </si>
+  <si>
+    <t>chēng</t>
+  </si>
+  <si>
+    <t>hong3</t>
+  </si>
+  <si>
+    <t>sein3</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">a pillar; extended to mean: resistance and support. Used in personal names.
+(composition: ⿰木堂; U+6A18).
+朱祐樘 jï-yiù-sẽin </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t>zhū yòuchēng</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Zhu Youcheng, personal name of The Hongzhi Emperor 弘治帝 fãng-jì-äi </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t>Hóngzhì Dì,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> the tenth Ming emporer, reigned from 1487 to 1505.
+樘柱 sẽin-chuî </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t>chēngzhù</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> to boycott; to resist.
+&lt;又&gt; hõng. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t>(See 樘 hõng.)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">door or window frame; &lt;m.&gt; a set or pair of windows or doors, similar to Western saloon doors, except that they cover the entire doorway.³⁹ʼ⁰
+(composition: ⿰木堂; U+6A18).
+两樘门[兩樘門] lēng-hõng-mõn </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t>liǎngtángmén</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> two pairs of doors.⁶ʼ⁰
+门樘[門樘] mõn-hõng </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t>méntáng</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> door frame.⁶
+窗樘 töng-hõng </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t>chuāngtáng</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> window frame.⁶
+四樘窗 xï-hõng-töng </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t>sìtángchuāng</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> four sets of windows.⁶ʼ⁰
+&lt;又&gt; sẽin. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t>(See 樘 sẽin.)</t>
     </r>
   </si>
 </sst>
@@ -2290,8 +2487,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:N24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30.75"/>
@@ -2790,7 +2987,7 @@
       </c>
       <c r="K15"/>
     </row>
-    <row r="16" spans="1:14" ht="138">
+    <row r="16" spans="1:14" ht="155.25">
       <c r="A16" s="2">
         <v>64</v>
       </c>
@@ -2823,7 +3020,7 @@
       </c>
       <c r="K16"/>
     </row>
-    <row r="17" spans="1:11" ht="86.25">
+    <row r="17" spans="1:11" ht="103.5">
       <c r="A17" s="19">
         <v>82</v>
       </c>
@@ -2915,7 +3112,7 @@
       </c>
       <c r="K19"/>
     </row>
-    <row r="20" spans="1:11" ht="138">
+    <row r="20" spans="1:11" ht="155.25">
       <c r="A20" s="2">
         <v>86</v>
       </c>
@@ -3010,23 +3207,64 @@
       </c>
       <c r="K22"/>
     </row>
-    <row r="23" spans="1:11">
-      <c r="A23" s="2"/>
-      <c r="B23" s="23"/>
-      <c r="C23" s="2"/>
-      <c r="D23" s="35"/>
+    <row r="23" spans="1:11" ht="189.75">
+      <c r="A23" s="2">
+        <v>75</v>
+      </c>
+      <c r="B23" s="23" t="s">
+        <v>121</v>
+      </c>
+      <c r="C23" s="2">
+        <v>15</v>
+      </c>
+      <c r="D23" s="35" t="s">
+        <v>122</v>
+      </c>
       <c r="E23" s="24"/>
-      <c r="F23" s="31"/>
-      <c r="G23" s="32"/>
-      <c r="H23" s="3"/>
-      <c r="I23" s="27"/>
-      <c r="J23" s="4"/>
+      <c r="F23" s="31" t="s">
+        <v>123</v>
+      </c>
+      <c r="G23" s="32" t="s">
+        <v>124</v>
+      </c>
+      <c r="H23" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="I23" s="27" t="s">
+        <v>127</v>
+      </c>
+      <c r="J23" s="4">
+        <v>6821</v>
+      </c>
     </row>
-    <row r="24" spans="1:11">
-      <c r="B24" s="21"/>
-      <c r="D24" s="42"/>
-      <c r="H24" s="15"/>
-      <c r="J24" s="4"/>
+    <row r="24" spans="1:11" ht="155.25">
+      <c r="A24" s="2">
+        <v>75</v>
+      </c>
+      <c r="B24" s="23" t="s">
+        <v>121</v>
+      </c>
+      <c r="C24" s="2">
+        <v>15</v>
+      </c>
+      <c r="D24" s="42" t="s">
+        <v>122</v>
+      </c>
+      <c r="F24" s="13" t="s">
+        <v>125</v>
+      </c>
+      <c r="G24" s="14" t="s">
+        <v>126</v>
+      </c>
+      <c r="H24" s="15" t="s">
+        <v>129</v>
+      </c>
+      <c r="I24" s="11" t="s">
+        <v>128</v>
+      </c>
+      <c r="J24" s="4">
+        <v>90022</v>
+      </c>
     </row>
   </sheetData>
   <sortState ref="A21:J23">
@@ -3034,10 +3272,11 @@
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
-  <webPublishItems count="5">
+  <webPublishItems count="6">
     <webPublishItem id="28518" divId="addendum_28518" sourceType="range" sourceRef="A1:K21" destinationFile="C:\Users\Gene\Documents\GitHub\chinfamilytree.github.io\hed\addenda\addendum.htm" title="Addendum"/>
     <webPublishItem id="15206" divId="addendum_15206" sourceType="range" sourceRef="A1:K22" destinationFile="C:\Users\Gene\Documents\GitHub\chinfamilytree.github.io\hed\addenda\addendum.htm" title="Addendum"/>
     <webPublishItem id="30801" divId="addendum_30801" sourceType="range" sourceRef="A1:K23" destinationFile="C:\Users\Gene\Documents\GitHub\chinfamilytree.github.io\hed\addenda\addendum.htm" title="Addendum"/>
+    <webPublishItem id="22021" divId="addendum_22021" sourceType="range" sourceRef="A1:K24" destinationFile="C:\Users\Gene\Documents\GitHub\chinfamilytree.github.io\hed\addenda\addendum.htm" title="Addendum"/>
     <webPublishItem id="213" divId="addendum_213" sourceType="range" sourceRef="A2:K4" destinationFile="C:\Users\Gene\Documents\GitHub\chinfamilytree.github.io\hed\addenda\addendum.htm"/>
     <webPublishItem id="21694" divId="addendum_21694" sourceType="range" sourceRef="A2:K21" destinationFile="C:\Users\Gene\Documents\GitHub\chinfamilytree.github.io\hed\addenda\addendum.htm" title="Addendum"/>
   </webPublishItems>

</xml_diff>

<commit_message>
changed ma-sang to ma-chang
</commit_message>
<xml_diff>
--- a/hed/addenda/addendum.xlsx
+++ b/hed/addenda/addendum.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="137">
   <si>
     <t>pit2</t>
   </si>
@@ -1871,6 +1871,26 @@
       </rPr>
       <t>(See 樘 sẽin.)</t>
     </r>
+  </si>
+  <si>
+    <t>子</t>
+  </si>
+  <si>
+    <t>孖</t>
+  </si>
+  <si>
+    <t>mä</t>
+  </si>
+  <si>
+    <t>mā</t>
+  </si>
+  <si>
+    <t>ma2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;台&gt; 孖 mä double; a pair; twin.
+&lt;台&gt; 孖生 read as mä-châng/ instead of mä-säng twins.
+</t>
   </si>
 </sst>
 </file>
@@ -2066,7 +2086,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2189,6 +2209,21 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2485,10 +2520,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N24"/>
+  <dimension ref="A1:N26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="K25" sqref="A1:K25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30.75"/>
@@ -3266,17 +3301,60 @@
         <v>90022</v>
       </c>
     </row>
+    <row r="25" spans="1:11" ht="51.75">
+      <c r="A25" s="9">
+        <v>39</v>
+      </c>
+      <c r="B25" s="21" t="s">
+        <v>131</v>
+      </c>
+      <c r="C25" s="9">
+        <v>6</v>
+      </c>
+      <c r="D25" s="42" t="s">
+        <v>132</v>
+      </c>
+      <c r="E25" s="43"/>
+      <c r="F25" s="44" t="s">
+        <v>133</v>
+      </c>
+      <c r="G25" s="45" t="s">
+        <v>134</v>
+      </c>
+      <c r="H25" s="46" t="s">
+        <v>136</v>
+      </c>
+      <c r="I25" s="47" t="s">
+        <v>135</v>
+      </c>
+      <c r="J25" s="9">
+        <v>10361</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" ht="17.25" customHeight="1">
+      <c r="A26" s="9"/>
+      <c r="B26" s="21"/>
+      <c r="C26" s="9"/>
+      <c r="D26" s="42"/>
+      <c r="E26" s="43"/>
+      <c r="F26" s="44"/>
+      <c r="G26" s="45"/>
+      <c r="H26" s="46"/>
+      <c r="I26" s="47"/>
+      <c r="J26" s="9"/>
+    </row>
   </sheetData>
   <sortState ref="A21:J23">
     <sortCondition ref="F21:F23"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
-  <webPublishItems count="6">
+  <webPublishItems count="7">
     <webPublishItem id="28518" divId="addendum_28518" sourceType="range" sourceRef="A1:K21" destinationFile="C:\Users\Gene\Documents\GitHub\chinfamilytree.github.io\hed\addenda\addendum.htm" title="Addendum"/>
     <webPublishItem id="15206" divId="addendum_15206" sourceType="range" sourceRef="A1:K22" destinationFile="C:\Users\Gene\Documents\GitHub\chinfamilytree.github.io\hed\addenda\addendum.htm" title="Addendum"/>
     <webPublishItem id="30801" divId="addendum_30801" sourceType="range" sourceRef="A1:K23" destinationFile="C:\Users\Gene\Documents\GitHub\chinfamilytree.github.io\hed\addenda\addendum.htm" title="Addendum"/>
     <webPublishItem id="22021" divId="addendum_22021" sourceType="range" sourceRef="A1:K24" destinationFile="C:\Users\Gene\Documents\GitHub\chinfamilytree.github.io\hed\addenda\addendum.htm" title="Addendum"/>
+    <webPublishItem id="18903" divId="addendum_18903" sourceType="range" sourceRef="A1:K25" destinationFile="C:\Users\Gene\Documents\GitHub\chinfamilytree.github.io\hed\addenda\addendum.htm" title="Gene Chin HED"/>
     <webPublishItem id="213" divId="addendum_213" sourceType="range" sourceRef="A2:K4" destinationFile="C:\Users\Gene\Documents\GitHub\chinfamilytree.github.io\hed\addenda\addendum.htm"/>
     <webPublishItem id="21694" divId="addendum_21694" sourceType="range" sourceRef="A2:K21" destinationFile="C:\Users\Gene\Documents\GitHub\chinfamilytree.github.io\hed\addenda\addendum.htm" title="Addendum"/>
   </webPublishItems>

</xml_diff>